<commit_message>
Ticket #2704: Excel to XML conversion log
</commit_message>
<xml_diff>
--- a/test/resources/seed-multivalues07.xlsx
+++ b/test/resources/seed-multivalues07.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150"/>
@@ -26,9 +26,6 @@
     <t>GWName</t>
   </si>
   <si>
-    <t>GWReference_year</t>
-  </si>
-  <si>
     <t>GWNo_of_horizon</t>
   </si>
   <si>
@@ -159,13 +156,16 @@
   </si>
   <si>
     <t>1;2;3</t>
+  </si>
+  <si>
+    <t>Reference_year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -223,6 +223,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -301,6 +306,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -335,6 +341,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -510,14 +517,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
@@ -560,7 +567,7 @@
     <col min="40" max="40" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="15">
+    <row r="1" spans="1:40" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,135 +578,135 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40">
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="S2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="S3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
-      <c r="S3" t="s">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
-      <c r="S4" t="s">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="S5" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40">
-      <c r="S5" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -710,31 +717,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>